<commit_message>
Remove notes of what was deleted
</commit_message>
<xml_diff>
--- a/6- Traceability link matrix/Traceability Link Matrix (P3).xlsx
+++ b/6- Traceability link matrix/Traceability Link Matrix (P3).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\CS414 Group Project\cs414-f20-public_class_TeamD\6- Traceability link matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C909690-94FB-4BCA-9322-04FE442564E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF15674-5393-4701-8A3E-0B4F1437EB9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44475" yWindow="4740" windowWidth="26400" windowHeight="11385" xr2:uid="{6F3B0F6D-D4FA-43ED-9BE5-68FBBAC2F32D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="81">
   <si>
     <t>User Stories</t>
   </si>
@@ -105,21 +105,12 @@
     <t>App</t>
   </si>
   <si>
-    <t>App.test</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
-    <t>Login.Test</t>
-  </si>
-  <si>
     <t>serviceWorker</t>
   </si>
   <si>
-    <t>setupTests</t>
-  </si>
-  <si>
     <t>CreateMatch</t>
   </si>
   <si>
@@ -150,12 +141,6 @@
     <t>ChessBoard</t>
   </si>
   <si>
-    <t>Greeting</t>
-  </si>
-  <si>
-    <t>GreetingController</t>
-  </si>
-  <si>
     <t>IllegalMoveException</t>
   </si>
   <si>
@@ -204,15 +189,6 @@
     <t xml:space="preserve">//Technically not a class. </t>
   </si>
   <si>
-    <t xml:space="preserve">//Technically a totally empty class. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">//Technically an empty class. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">//Empty class. </t>
-  </si>
-  <si>
     <t>Ping</t>
   </si>
   <si>
@@ -297,16 +273,10 @@
     <t>OngoingMatchesTest</t>
   </si>
   <si>
-    <t>TeamDApplicationTest</t>
-  </si>
-  <si>
     <t xml:space="preserve">//Mostly empty and unused. </t>
   </si>
   <si>
     <t xml:space="preserve">//Some of these are "would/will be" instead of "are", because not everything is implemented yet. </t>
-  </si>
-  <si>
-    <t>DELETED</t>
   </si>
 </sst>
 </file>
@@ -683,11 +653,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C21C376-BCAA-4BB5-9BB8-5CF377B37712}">
-  <dimension ref="A1:BT27"/>
+  <dimension ref="A1:BN27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BT20" sqref="BT20"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,84 +667,78 @@
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="21" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="16" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="10" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="21" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="16" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -795,202 +759,184 @@
         <v>23</v>
       </c>
       <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>27</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" t="s">
         <v>52</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" t="s">
         <v>53</v>
       </c>
-      <c r="P2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" t="s">
-        <v>59</v>
-      </c>
-      <c r="U2" t="s">
-        <v>60</v>
-      </c>
-      <c r="V2" t="s">
-        <v>31</v>
-      </c>
-      <c r="W2" t="s">
-        <v>34</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>35</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>37</v>
       </c>
       <c r="Z2" t="s">
         <v>36</v>
       </c>
       <c r="AA2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="AB2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD2" t="s">
         <v>41</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>42</v>
       </c>
       <c r="AE2" t="s">
         <v>43</v>
       </c>
       <c r="AF2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU2" t="s">
         <v>44</v>
       </c>
-      <c r="AG2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="AV2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AX2" t="s">
         <v>62</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AY2" t="s">
         <v>63</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AZ2" t="s">
         <v>64</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="BA2" t="s">
         <v>65</v>
       </c>
-      <c r="AN2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO2" t="s">
+      <c r="BB2" t="s">
         <v>66</v>
       </c>
-      <c r="AP2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AY2" t="s">
+      <c r="BC2" t="s">
         <v>67</v>
       </c>
-      <c r="AZ2" t="s">
-        <v>49</v>
-      </c>
-      <c r="BA2" t="s">
+      <c r="BD2" t="s">
         <v>68</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BE2" t="s">
         <v>69</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BF2" t="s">
         <v>70</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BG2" t="s">
         <v>71</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BH2" t="s">
         <v>72</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BI2" t="s">
         <v>73</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BJ2" t="s">
         <v>74</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BK2" t="s">
         <v>75</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="BL2" t="s">
         <v>76</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="BM2" t="s">
         <v>77</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="BN2" t="s">
         <v>78</v>
       </c>
-      <c r="BL2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>81</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>82</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>83</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>84</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>85</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>86</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>87</v>
-      </c>
     </row>
-    <row r="3" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -998,15 +944,15 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="H3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -1016,12 +962,12 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
+      <c r="S3" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
-      <c r="V3" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
@@ -1042,47 +988,41 @@
       <c r="AN3" s="3"/>
       <c r="AO3" s="3"/>
       <c r="AP3" s="3"/>
-      <c r="AQ3" s="3"/>
-      <c r="AR3" s="3"/>
+      <c r="AQ3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AS3" s="3"/>
-      <c r="AT3" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AT3" s="3"/>
       <c r="AU3" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AV3" s="3"/>
       <c r="AW3" s="3"/>
-      <c r="AX3" s="3"/>
+      <c r="AX3" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AY3" s="3"/>
-      <c r="AZ3" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AZ3" s="3"/>
       <c r="BA3" s="3"/>
       <c r="BB3" s="3"/>
-      <c r="BC3" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="BC3" s="3"/>
       <c r="BD3" s="3"/>
       <c r="BE3" s="3"/>
       <c r="BF3" s="3"/>
       <c r="BG3" s="3"/>
       <c r="BH3" s="3"/>
-      <c r="BI3" s="3"/>
       <c r="BJ3" s="3"/>
       <c r="BK3" s="3"/>
       <c r="BL3" s="3"/>
-      <c r="BM3" s="3"/>
-      <c r="BO3" s="3"/>
-      <c r="BP3" s="3"/>
-      <c r="BQ3" s="3"/>
-      <c r="BR3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BS3" s="3"/>
-      <c r="BT3" s="3"/>
+      <c r="BM3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BN3" s="3"/>
     </row>
-    <row r="4" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1144,46 +1084,40 @@
       <c r="BF4" s="3"/>
       <c r="BG4" s="3"/>
       <c r="BH4" s="3"/>
-      <c r="BI4" s="3"/>
       <c r="BJ4" s="3"/>
       <c r="BK4" s="3"/>
       <c r="BL4" s="3"/>
       <c r="BM4" s="3"/>
-      <c r="BO4" s="3"/>
-      <c r="BP4" s="3"/>
-      <c r="BQ4" s="3"/>
-      <c r="BR4" s="3"/>
-      <c r="BS4" s="3"/>
-      <c r="BT4" s="3"/>
+      <c r="BN4" s="3"/>
     </row>
-    <row r="5" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="M5" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
@@ -1208,24 +1142,24 @@
       <c r="AL5" s="3"/>
       <c r="AM5" s="3"/>
       <c r="AN5" s="3"/>
-      <c r="AO5" s="3"/>
-      <c r="AP5" s="3"/>
+      <c r="AO5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP5" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AQ5" s="3"/>
-      <c r="AR5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AS5" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AR5" s="3"/>
+      <c r="AS5" s="3"/>
       <c r="AT5" s="3"/>
-      <c r="AU5" s="3"/>
+      <c r="AU5" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AV5" s="3"/>
       <c r="AW5" s="3"/>
       <c r="AX5" s="3"/>
       <c r="AY5" s="3"/>
-      <c r="AZ5" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AZ5" s="3"/>
       <c r="BA5" s="3"/>
       <c r="BB5" s="3"/>
       <c r="BC5" s="3"/>
@@ -1234,64 +1168,58 @@
       <c r="BF5" s="3"/>
       <c r="BG5" s="3"/>
       <c r="BH5" s="3"/>
-      <c r="BI5" s="3"/>
       <c r="BJ5" s="3"/>
       <c r="BK5" s="3"/>
       <c r="BL5" s="3"/>
       <c r="BM5" s="3"/>
-      <c r="BO5" s="3"/>
-      <c r="BP5" s="3"/>
-      <c r="BQ5" s="3"/>
-      <c r="BR5" s="3"/>
-      <c r="BS5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BT5" s="3"/>
+      <c r="BN5" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="6" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="N6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="Q6" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
@@ -1302,112 +1230,106 @@
       <c r="AD6" s="3"/>
       <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
+      <c r="AG6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AJ6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM6" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
       <c r="AN6" s="3"/>
       <c r="AO6" s="3"/>
       <c r="AP6" s="3"/>
       <c r="AQ6" s="3"/>
       <c r="AR6" s="3"/>
-      <c r="AS6" s="3"/>
-      <c r="AT6" s="3"/>
-      <c r="AU6" s="3"/>
-      <c r="AV6" s="3"/>
-      <c r="AW6" s="3"/>
+      <c r="AS6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW6" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AX6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AY6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AZ6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BC6" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AY6" s="3"/>
+      <c r="AZ6" s="3"/>
+      <c r="BA6" s="3"/>
+      <c r="BB6" s="3"/>
+      <c r="BC6" s="3"/>
       <c r="BD6" s="3"/>
       <c r="BE6" s="3"/>
       <c r="BF6" s="3"/>
       <c r="BG6" s="3"/>
       <c r="BH6" s="3"/>
-      <c r="BI6" s="3"/>
-      <c r="BJ6" s="3"/>
+      <c r="BJ6" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="BK6" s="3"/>
       <c r="BL6" s="3"/>
       <c r="BM6" s="3"/>
-      <c r="BO6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BP6" s="3"/>
-      <c r="BQ6" s="3"/>
-      <c r="BR6" s="3"/>
-      <c r="BS6" s="3"/>
-      <c r="BT6" s="3"/>
+      <c r="BN6" s="3"/>
     </row>
-    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="N7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="Q7" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
@@ -1418,21 +1340,21 @@
       <c r="AD7" s="3"/>
       <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="3"/>
+      <c r="AG7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AJ7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM7" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
       <c r="AN7" s="3"/>
       <c r="AO7" s="3"/>
       <c r="AP7" s="3"/>
@@ -1440,43 +1362,37 @@
       <c r="AR7" s="3"/>
       <c r="AS7" s="3"/>
       <c r="AT7" s="3"/>
-      <c r="AU7" s="3"/>
-      <c r="AV7" s="3"/>
-      <c r="AW7" s="3"/>
-      <c r="AX7" s="3"/>
+      <c r="AU7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AX7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AY7" s="3"/>
-      <c r="AZ7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BC7" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AZ7" s="3"/>
+      <c r="BA7" s="3"/>
+      <c r="BB7" s="3"/>
+      <c r="BC7" s="3"/>
       <c r="BD7" s="3"/>
       <c r="BE7" s="3"/>
       <c r="BF7" s="3"/>
       <c r="BG7" s="3"/>
       <c r="BH7" s="3"/>
-      <c r="BI7" s="3"/>
-      <c r="BJ7" s="3"/>
+      <c r="BJ7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="BK7" s="3"/>
       <c r="BL7" s="3"/>
       <c r="BM7" s="3"/>
-      <c r="BO7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BP7" s="3"/>
-      <c r="BQ7" s="3"/>
-      <c r="BR7" s="3"/>
-      <c r="BS7" s="3"/>
-      <c r="BT7" s="3"/>
+      <c r="BN7" s="3"/>
     </row>
-    <row r="8" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -1538,19 +1454,13 @@
       <c r="BF8" s="3"/>
       <c r="BG8" s="3"/>
       <c r="BH8" s="3"/>
-      <c r="BI8" s="3"/>
       <c r="BJ8" s="3"/>
       <c r="BK8" s="3"/>
       <c r="BL8" s="3"/>
       <c r="BM8" s="3"/>
-      <c r="BO8" s="3"/>
-      <c r="BP8" s="3"/>
-      <c r="BQ8" s="3"/>
-      <c r="BR8" s="3"/>
-      <c r="BS8" s="3"/>
-      <c r="BT8" s="3"/>
+      <c r="BN8" s="3"/>
     </row>
-    <row r="9" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1612,19 +1522,13 @@
       <c r="BF9" s="3"/>
       <c r="BG9" s="3"/>
       <c r="BH9" s="3"/>
-      <c r="BI9" s="3"/>
       <c r="BJ9" s="3"/>
       <c r="BK9" s="3"/>
       <c r="BL9" s="3"/>
       <c r="BM9" s="3"/>
-      <c r="BO9" s="3"/>
-      <c r="BP9" s="3"/>
-      <c r="BQ9" s="3"/>
-      <c r="BR9" s="3"/>
-      <c r="BS9" s="3"/>
-      <c r="BT9" s="3"/>
+      <c r="BN9" s="3"/>
     </row>
-    <row r="10" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -1632,15 +1536,15 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="H10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -1650,12 +1554,12 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
+      <c r="S10" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
-      <c r="V10" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
@@ -1670,63 +1574,57 @@
       <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
       <c r="AJ10" s="3"/>
-      <c r="AK10" s="3"/>
-      <c r="AL10" s="3"/>
-      <c r="AM10" s="3"/>
+      <c r="AK10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM10" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AN10" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AO10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR10" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
       <c r="AT10" s="3"/>
-      <c r="AU10" s="3"/>
+      <c r="AU10" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AV10" s="3"/>
       <c r="AW10" s="3"/>
-      <c r="AX10" s="3"/>
+      <c r="AX10" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AY10" s="3"/>
-      <c r="AZ10" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AZ10" s="3"/>
       <c r="BA10" s="3"/>
       <c r="BB10" s="3"/>
-      <c r="BC10" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="BC10" s="3"/>
       <c r="BD10" s="3"/>
       <c r="BE10" s="3"/>
       <c r="BF10" s="3"/>
       <c r="BG10" s="3"/>
       <c r="BH10" s="3"/>
-      <c r="BI10" s="3"/>
       <c r="BJ10" s="3"/>
-      <c r="BK10" s="3"/>
-      <c r="BL10" s="3"/>
+      <c r="BK10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BL10" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="BM10" s="3"/>
-      <c r="BO10" s="3"/>
-      <c r="BP10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BQ10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BR10" s="3"/>
-      <c r="BS10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BT10" s="3"/>
+      <c r="BN10" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="11" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -1734,65 +1632,65 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="M11" s="3"/>
-      <c r="N11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
+      <c r="S11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="V11" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="X11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-      <c r="AC11" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AD11" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AE11" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AF11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI11" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3"/>
       <c r="AL11" s="3"/>
@@ -1804,75 +1702,69 @@
       <c r="AR11" s="3"/>
       <c r="AS11" s="3"/>
       <c r="AT11" s="3"/>
-      <c r="AU11" s="3"/>
+      <c r="AU11" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AV11" s="3"/>
       <c r="AW11" s="3"/>
-      <c r="AX11" s="3"/>
-      <c r="AY11" s="3"/>
+      <c r="AX11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AY11" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AZ11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA11" s="3"/>
-      <c r="BB11" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="BA11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BB11" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="BC11" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="BD11" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="BE11" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="BF11" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="BG11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BH11" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="BH11" s="3"/>
       <c r="BI11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BJ11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BK11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BL11" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="BJ11" s="3"/>
+      <c r="BK11" s="3"/>
+      <c r="BL11" s="3"/>
       <c r="BM11" s="3"/>
-      <c r="BN11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BO11" s="3"/>
-      <c r="BP11" s="3"/>
-      <c r="BQ11" s="3"/>
-      <c r="BR11" s="3"/>
-      <c r="BS11" s="3"/>
-      <c r="BT11" s="3"/>
+      <c r="BN11" s="3"/>
     </row>
-    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1925,19 +1817,13 @@
       <c r="BF12" s="3"/>
       <c r="BG12" s="3"/>
       <c r="BH12" s="3"/>
-      <c r="BI12" s="3"/>
       <c r="BJ12" s="3"/>
       <c r="BK12" s="3"/>
       <c r="BL12" s="3"/>
       <c r="BM12" s="3"/>
-      <c r="BO12" s="3"/>
-      <c r="BP12" s="3"/>
-      <c r="BQ12" s="3"/>
-      <c r="BR12" s="3"/>
-      <c r="BS12" s="3"/>
-      <c r="BT12" s="3"/>
+      <c r="BN12" s="3"/>
     </row>
-    <row r="13" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -1999,19 +1885,13 @@
       <c r="BF13" s="3"/>
       <c r="BG13" s="3"/>
       <c r="BH13" s="3"/>
-      <c r="BI13" s="3"/>
       <c r="BJ13" s="3"/>
       <c r="BK13" s="3"/>
       <c r="BL13" s="3"/>
       <c r="BM13" s="3"/>
-      <c r="BO13" s="3"/>
-      <c r="BP13" s="3"/>
-      <c r="BQ13" s="3"/>
-      <c r="BR13" s="3"/>
-      <c r="BS13" s="3"/>
-      <c r="BT13" s="3"/>
+      <c r="BN13" s="3"/>
     </row>
-    <row r="14" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -2019,12 +1899,12 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -2061,20 +1941,20 @@
       <c r="AP14" s="3"/>
       <c r="AQ14" s="3"/>
       <c r="AR14" s="3"/>
-      <c r="AS14" s="3"/>
-      <c r="AT14" s="3"/>
-      <c r="AU14" s="3"/>
+      <c r="AS14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU14" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AV14" s="3"/>
       <c r="AW14" s="3"/>
-      <c r="AX14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AY14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AZ14" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AX14" s="3"/>
+      <c r="AY14" s="3"/>
+      <c r="AZ14" s="3"/>
       <c r="BA14" s="3"/>
       <c r="BB14" s="3"/>
       <c r="BC14" s="3"/>
@@ -2083,19 +1963,13 @@
       <c r="BF14" s="3"/>
       <c r="BG14" s="3"/>
       <c r="BH14" s="3"/>
-      <c r="BI14" s="3"/>
       <c r="BJ14" s="3"/>
       <c r="BK14" s="3"/>
       <c r="BL14" s="3"/>
       <c r="BM14" s="3"/>
-      <c r="BO14" s="3"/>
-      <c r="BP14" s="3"/>
-      <c r="BQ14" s="3"/>
-      <c r="BR14" s="3"/>
-      <c r="BS14" s="3"/>
-      <c r="BT14" s="3"/>
+      <c r="BN14" s="3"/>
     </row>
-    <row r="15" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -2103,69 +1977,69 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="K15" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
-      <c r="N15" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
+      <c r="S15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="V15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="X15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Y15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AA15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AB15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AC15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AD15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AE15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AF15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI15" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
       <c r="AJ15" s="3"/>
       <c r="AK15" s="3"/>
       <c r="AL15" s="3"/>
@@ -2177,60 +2051,54 @@
       <c r="AR15" s="3"/>
       <c r="AS15" s="3"/>
       <c r="AT15" s="3"/>
-      <c r="AU15" s="3"/>
+      <c r="AU15" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AV15" s="3"/>
       <c r="AW15" s="3"/>
-      <c r="AX15" s="3"/>
-      <c r="AY15" s="3"/>
+      <c r="AX15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AY15" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AZ15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA15" s="3"/>
-      <c r="BB15" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="BA15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BB15" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="BC15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="BD15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="BE15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="BF15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="BG15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="BH15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="BI15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BJ15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BK15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BL15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BM15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BN15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BO15" s="3"/>
-      <c r="BP15" s="3"/>
-      <c r="BQ15" s="3"/>
-      <c r="BR15" s="3"/>
-      <c r="BS15" s="3"/>
-      <c r="BT15" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="BJ15" s="3"/>
+      <c r="BK15" s="3"/>
+      <c r="BL15" s="3"/>
+      <c r="BM15" s="3"/>
+      <c r="BN15" s="3"/>
     </row>
-    <row r="16" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -2242,12 +2110,12 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="K16" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -2255,19 +2123,19 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
+      <c r="V16" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
-      <c r="Y16" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
+      <c r="AA16" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
-      <c r="AD16" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AD16" s="3"/>
       <c r="AE16" s="3"/>
       <c r="AF16" s="3"/>
       <c r="AG16" s="3"/>
@@ -2284,39 +2152,33 @@
       <c r="AR16" s="3"/>
       <c r="AS16" s="3"/>
       <c r="AT16" s="3"/>
-      <c r="AU16" s="3"/>
+      <c r="AU16" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AV16" s="3"/>
       <c r="AW16" s="3"/>
       <c r="AX16" s="3"/>
       <c r="AY16" s="3"/>
-      <c r="AZ16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA16" s="3"/>
+      <c r="AZ16" s="3"/>
+      <c r="BA16" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="BB16" s="3"/>
-      <c r="BC16" s="3"/>
+      <c r="BC16" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="BD16" s="3"/>
       <c r="BE16" s="3"/>
-      <c r="BF16" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="BF16" s="3"/>
       <c r="BG16" s="3"/>
-      <c r="BH16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BI16" s="3"/>
+      <c r="BH16" s="3"/>
       <c r="BJ16" s="3"/>
       <c r="BK16" s="3"/>
       <c r="BL16" s="3"/>
       <c r="BM16" s="3"/>
-      <c r="BO16" s="3"/>
-      <c r="BP16" s="3"/>
-      <c r="BQ16" s="3"/>
-      <c r="BR16" s="3"/>
-      <c r="BS16" s="3"/>
-      <c r="BT16" s="3"/>
+      <c r="BN16" s="3"/>
     </row>
-    <row r="17" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -2328,12 +2190,12 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="K17" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
@@ -2366,14 +2228,14 @@
       <c r="AR17" s="3"/>
       <c r="AS17" s="3"/>
       <c r="AT17" s="3"/>
-      <c r="AU17" s="3"/>
+      <c r="AU17" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AV17" s="3"/>
       <c r="AW17" s="3"/>
       <c r="AX17" s="3"/>
       <c r="AY17" s="3"/>
-      <c r="AZ17" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AZ17" s="3"/>
       <c r="BA17" s="3"/>
       <c r="BB17" s="3"/>
       <c r="BC17" s="3"/>
@@ -2388,70 +2250,31 @@
       <c r="BL17" s="3"/>
       <c r="BM17" s="3"/>
       <c r="BN17" s="3"/>
-      <c r="BO17" s="3"/>
-      <c r="BP17" s="3"/>
-      <c r="BQ17" s="3"/>
-      <c r="BR17" s="3"/>
-      <c r="BS17" s="3"/>
-      <c r="BT17" s="3"/>
     </row>
-    <row r="20" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
-      <c r="B20" t="s">
-        <v>90</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AV20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AW20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BT20" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="B20"/>
     </row>
-    <row r="22" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
     </row>
-    <row r="23" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="N23" t="s">
-        <v>89</v>
+    <row r="23" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="G24" t="s">
-        <v>56</v>
-      </c>
-      <c r="M24" t="s">
-        <v>58</v>
+    <row r="25" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="H25" t="s">
-        <v>55</v>
-      </c>
-      <c r="L25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="J26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="K27" t="s">
-        <v>88</v>
+    <row r="27" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delete unused Registration page
</commit_message>
<xml_diff>
--- a/6- Traceability link matrix/Traceability Link Matrix (P3).xlsx
+++ b/6- Traceability link matrix/Traceability Link Matrix (P3).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\CS414 Group Project\cs414-f20-public_class_TeamD\6- Traceability link matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF15674-5393-4701-8A3E-0B4F1437EB9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCBFF45-FCDA-4CFD-B45E-121628C9C769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44475" yWindow="4740" windowWidth="26400" windowHeight="11385" xr2:uid="{6F3B0F6D-D4FA-43ED-9BE5-68FBBAC2F32D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="80">
   <si>
     <t>User Stories</t>
   </si>
@@ -271,9 +271,6 @@
   </si>
   <si>
     <t>OngoingMatchesTest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//Mostly empty and unused. </t>
   </si>
   <si>
     <t xml:space="preserve">//Some of these are "would/will be" instead of "are", because not everything is implemented yet. </t>
@@ -653,11 +650,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C21C376-BCAA-4BB5-9BB8-5CF377B37712}">
-  <dimension ref="A1:BN27"/>
+  <dimension ref="A1:BM25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B20" sqref="B20"/>
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,76 +666,75 @@
     <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="21" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="16" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="21" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="16" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -762,181 +758,178 @@
         <v>9</v>
       </c>
       <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" t="s">
-        <v>31</v>
-      </c>
-      <c r="U2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W2" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>30</v>
-      </c>
       <c r="AQ2" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="AR2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AS2" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="AT2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="AU2" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="AV2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AW2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AX2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AY2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AZ2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="BA2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="BB2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BC2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="BD2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BE2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="BF2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="BG2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="BH2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="BI2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="BJ2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="BK2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="BL2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="BM2" t="s">
-        <v>77</v>
-      </c>
-      <c r="BN2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -961,10 +954,10 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="R3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="S3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
@@ -987,23 +980,23 @@
       <c r="AM3" s="3"/>
       <c r="AN3" s="3"/>
       <c r="AO3" s="3"/>
-      <c r="AP3" s="3"/>
+      <c r="AP3" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AQ3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AR3" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AR3" s="3"/>
       <c r="AS3" s="3"/>
-      <c r="AT3" s="3"/>
-      <c r="AU3" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AT3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU3" s="3"/>
       <c r="AV3" s="3"/>
-      <c r="AW3" s="3"/>
-      <c r="AX3" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AW3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AX3" s="3"/>
       <c r="AY3" s="3"/>
       <c r="AZ3" s="3"/>
       <c r="BA3" s="3"/>
@@ -1013,16 +1006,15 @@
       <c r="BE3" s="3"/>
       <c r="BF3" s="3"/>
       <c r="BG3" s="3"/>
-      <c r="BH3" s="3"/>
+      <c r="BI3" s="3"/>
       <c r="BJ3" s="3"/>
       <c r="BK3" s="3"/>
-      <c r="BL3" s="3"/>
-      <c r="BM3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BN3" s="3"/>
+      <c r="BL3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BM3" s="3"/>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1083,14 +1075,13 @@
       <c r="BE4" s="3"/>
       <c r="BF4" s="3"/>
       <c r="BG4" s="3"/>
-      <c r="BH4" s="3"/>
+      <c r="BI4" s="3"/>
       <c r="BJ4" s="3"/>
       <c r="BK4" s="3"/>
       <c r="BL4" s="3"/>
       <c r="BM4" s="3"/>
-      <c r="BN4" s="3"/>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1111,10 +1102,10 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="L5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -1141,20 +1132,20 @@
       <c r="AK5" s="3"/>
       <c r="AL5" s="3"/>
       <c r="AM5" s="3"/>
-      <c r="AN5" s="3"/>
+      <c r="AN5" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AO5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AP5" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AP5" s="3"/>
       <c r="AQ5" s="3"/>
       <c r="AR5" s="3"/>
       <c r="AS5" s="3"/>
-      <c r="AT5" s="3"/>
-      <c r="AU5" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AT5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU5" s="3"/>
       <c r="AV5" s="3"/>
       <c r="AW5" s="3"/>
       <c r="AX5" s="3"/>
@@ -1167,16 +1158,15 @@
       <c r="BE5" s="3"/>
       <c r="BF5" s="3"/>
       <c r="BG5" s="3"/>
-      <c r="BH5" s="3"/>
+      <c r="BI5" s="3"/>
       <c r="BJ5" s="3"/>
       <c r="BK5" s="3"/>
       <c r="BL5" s="3"/>
-      <c r="BM5" s="3"/>
-      <c r="BN5" s="3" t="s">
+      <c r="BM5" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1198,7 +1188,9 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="M6" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="N6" s="3" t="s">
         <v>46</v>
       </c>
@@ -1214,9 +1206,7 @@
       <c r="R6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="S6" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
@@ -1229,7 +1219,9 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
       <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
+      <c r="AF6" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AG6" s="3" t="s">
         <v>46</v>
       </c>
@@ -1239,9 +1231,7 @@
       <c r="AI6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AJ6" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AJ6" s="3"/>
       <c r="AK6" s="3"/>
       <c r="AL6" s="3"/>
       <c r="AM6" s="3"/>
@@ -1249,7 +1239,9 @@
       <c r="AO6" s="3"/>
       <c r="AP6" s="3"/>
       <c r="AQ6" s="3"/>
-      <c r="AR6" s="3"/>
+      <c r="AR6" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AS6" s="3" t="s">
         <v>46</v>
       </c>
@@ -1265,9 +1257,7 @@
       <c r="AW6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AX6" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AX6" s="3"/>
       <c r="AY6" s="3"/>
       <c r="AZ6" s="3"/>
       <c r="BA6" s="3"/>
@@ -1277,16 +1267,15 @@
       <c r="BE6" s="3"/>
       <c r="BF6" s="3"/>
       <c r="BG6" s="3"/>
-      <c r="BH6" s="3"/>
-      <c r="BJ6" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="BI6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BJ6" s="3"/>
       <c r="BK6" s="3"/>
       <c r="BL6" s="3"/>
       <c r="BM6" s="3"/>
-      <c r="BN6" s="3"/>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -1308,7 +1297,9 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="M7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="N7" s="3" t="s">
         <v>46</v>
       </c>
@@ -1324,9 +1315,7 @@
       <c r="R7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="S7" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
@@ -1339,7 +1328,9 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
       <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
+      <c r="AF7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AG7" s="3" t="s">
         <v>46</v>
       </c>
@@ -1349,9 +1340,7 @@
       <c r="AI7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AJ7" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AJ7" s="3"/>
       <c r="AK7" s="3"/>
       <c r="AL7" s="3"/>
       <c r="AM7" s="3"/>
@@ -1361,7 +1350,9 @@
       <c r="AQ7" s="3"/>
       <c r="AR7" s="3"/>
       <c r="AS7" s="3"/>
-      <c r="AT7" s="3"/>
+      <c r="AT7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AU7" s="3" t="s">
         <v>46</v>
       </c>
@@ -1371,9 +1362,7 @@
       <c r="AW7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AX7" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AX7" s="3"/>
       <c r="AY7" s="3"/>
       <c r="AZ7" s="3"/>
       <c r="BA7" s="3"/>
@@ -1383,16 +1372,15 @@
       <c r="BE7" s="3"/>
       <c r="BF7" s="3"/>
       <c r="BG7" s="3"/>
-      <c r="BH7" s="3"/>
-      <c r="BJ7" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="BI7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BJ7" s="3"/>
       <c r="BK7" s="3"/>
       <c r="BL7" s="3"/>
       <c r="BM7" s="3"/>
-      <c r="BN7" s="3"/>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -1453,14 +1441,13 @@
       <c r="BE8" s="3"/>
       <c r="BF8" s="3"/>
       <c r="BG8" s="3"/>
-      <c r="BH8" s="3"/>
+      <c r="BI8" s="3"/>
       <c r="BJ8" s="3"/>
       <c r="BK8" s="3"/>
       <c r="BL8" s="3"/>
       <c r="BM8" s="3"/>
-      <c r="BN8" s="3"/>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1521,14 +1508,13 @@
       <c r="BE9" s="3"/>
       <c r="BF9" s="3"/>
       <c r="BG9" s="3"/>
-      <c r="BH9" s="3"/>
+      <c r="BI9" s="3"/>
       <c r="BJ9" s="3"/>
       <c r="BK9" s="3"/>
       <c r="BL9" s="3"/>
       <c r="BM9" s="3"/>
-      <c r="BN9" s="3"/>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -1553,10 +1539,10 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="R10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
@@ -1573,7 +1559,9 @@
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
-      <c r="AJ10" s="3"/>
+      <c r="AJ10" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AK10" s="3" t="s">
         <v>46</v>
       </c>
@@ -1586,22 +1574,20 @@
       <c r="AN10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AO10" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AO10" s="3"/>
       <c r="AP10" s="3"/>
       <c r="AQ10" s="3"/>
       <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
-      <c r="AT10" s="3"/>
-      <c r="AU10" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AT10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU10" s="3"/>
       <c r="AV10" s="3"/>
-      <c r="AW10" s="3"/>
-      <c r="AX10" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AW10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AX10" s="3"/>
       <c r="AY10" s="3"/>
       <c r="AZ10" s="3"/>
       <c r="BA10" s="3"/>
@@ -1611,20 +1597,19 @@
       <c r="BE10" s="3"/>
       <c r="BF10" s="3"/>
       <c r="BG10" s="3"/>
-      <c r="BH10" s="3"/>
-      <c r="BJ10" s="3"/>
+      <c r="BI10" s="3"/>
+      <c r="BJ10" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="BK10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="BL10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BM10" s="3"/>
-      <c r="BN10" s="3" t="s">
+      <c r="BL10" s="3"/>
+      <c r="BM10" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -1639,19 +1624,21 @@
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="K11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
+      <c r="R11" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="S11" s="3" t="s">
         <v>46</v>
       </c>
@@ -1664,12 +1651,12 @@
       <c r="V11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="W11" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
+      <c r="Z11" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AA11" s="3" t="s">
         <v>46</v>
       </c>
@@ -1685,9 +1672,7 @@
       <c r="AE11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AF11" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AF11" s="3"/>
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
       <c r="AI11" s="3"/>
@@ -1701,12 +1686,14 @@
       <c r="AQ11" s="3"/>
       <c r="AR11" s="3"/>
       <c r="AS11" s="3"/>
-      <c r="AT11" s="3"/>
-      <c r="AU11" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AT11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU11" s="3"/>
       <c r="AV11" s="3"/>
-      <c r="AW11" s="3"/>
+      <c r="AW11" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AX11" s="3" t="s">
         <v>46</v>
       </c>
@@ -1734,20 +1721,17 @@
       <c r="BF11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="BG11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BH11" s="3"/>
-      <c r="BI11" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="BG11" s="3"/>
+      <c r="BH11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BI11" s="3"/>
       <c r="BJ11" s="3"/>
       <c r="BK11" s="3"/>
       <c r="BL11" s="3"/>
       <c r="BM11" s="3"/>
-      <c r="BN11" s="3"/>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -1816,14 +1800,13 @@
       <c r="BE12" s="3"/>
       <c r="BF12" s="3"/>
       <c r="BG12" s="3"/>
-      <c r="BH12" s="3"/>
+      <c r="BI12" s="3"/>
       <c r="BJ12" s="3"/>
       <c r="BK12" s="3"/>
       <c r="BL12" s="3"/>
       <c r="BM12" s="3"/>
-      <c r="BN12" s="3"/>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -1884,14 +1867,13 @@
       <c r="BE13" s="3"/>
       <c r="BF13" s="3"/>
       <c r="BG13" s="3"/>
-      <c r="BH13" s="3"/>
+      <c r="BI13" s="3"/>
       <c r="BJ13" s="3"/>
       <c r="BK13" s="3"/>
       <c r="BL13" s="3"/>
       <c r="BM13" s="3"/>
-      <c r="BN13" s="3"/>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -1940,16 +1922,16 @@
       <c r="AO14" s="3"/>
       <c r="AP14" s="3"/>
       <c r="AQ14" s="3"/>
-      <c r="AR14" s="3"/>
+      <c r="AR14" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AS14" s="3" t="s">
         <v>46</v>
       </c>
       <c r="AT14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AU14" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AU14" s="3"/>
       <c r="AV14" s="3"/>
       <c r="AW14" s="3"/>
       <c r="AX14" s="3"/>
@@ -1962,14 +1944,13 @@
       <c r="BE14" s="3"/>
       <c r="BF14" s="3"/>
       <c r="BG14" s="3"/>
-      <c r="BH14" s="3"/>
+      <c r="BI14" s="3"/>
       <c r="BJ14" s="3"/>
       <c r="BK14" s="3"/>
       <c r="BL14" s="3"/>
       <c r="BM14" s="3"/>
-      <c r="BN14" s="3"/>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -1984,17 +1965,19 @@
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="J15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
+      <c r="R15" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="S15" s="3" t="s">
         <v>46</v>
       </c>
@@ -2034,9 +2017,7 @@
       <c r="AE15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AF15" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
       <c r="AI15" s="3"/>
@@ -2050,12 +2031,14 @@
       <c r="AQ15" s="3"/>
       <c r="AR15" s="3"/>
       <c r="AS15" s="3"/>
-      <c r="AT15" s="3"/>
-      <c r="AU15" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AT15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU15" s="3"/>
       <c r="AV15" s="3"/>
-      <c r="AW15" s="3"/>
+      <c r="AW15" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="AX15" s="3" t="s">
         <v>46</v>
       </c>
@@ -2089,16 +2072,13 @@
       <c r="BH15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="BI15" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="BI15" s="3"/>
       <c r="BJ15" s="3"/>
       <c r="BK15" s="3"/>
       <c r="BL15" s="3"/>
       <c r="BM15" s="3"/>
-      <c r="BN15" s="3"/>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -2109,10 +2089,10 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="J16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -2122,17 +2102,17 @@
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="U16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="Z16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
@@ -2151,34 +2131,33 @@
       <c r="AQ16" s="3"/>
       <c r="AR16" s="3"/>
       <c r="AS16" s="3"/>
-      <c r="AT16" s="3"/>
-      <c r="AU16" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AT16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU16" s="3"/>
       <c r="AV16" s="3"/>
       <c r="AW16" s="3"/>
       <c r="AX16" s="3"/>
       <c r="AY16" s="3"/>
-      <c r="AZ16" s="3"/>
-      <c r="BA16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BB16" s="3"/>
-      <c r="BC16" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AZ16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA16" s="3"/>
+      <c r="BB16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC16" s="3"/>
       <c r="BD16" s="3"/>
       <c r="BE16" s="3"/>
       <c r="BF16" s="3"/>
       <c r="BG16" s="3"/>
-      <c r="BH16" s="3"/>
+      <c r="BI16" s="3"/>
       <c r="BJ16" s="3"/>
       <c r="BK16" s="3"/>
       <c r="BL16" s="3"/>
       <c r="BM16" s="3"/>
-      <c r="BN16" s="3"/>
     </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -2189,10 +2168,10 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="J17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -2227,10 +2206,10 @@
       <c r="AQ17" s="3"/>
       <c r="AR17" s="3"/>
       <c r="AS17" s="3"/>
-      <c r="AT17" s="3"/>
-      <c r="AU17" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AT17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU17" s="3"/>
       <c r="AV17" s="3"/>
       <c r="AW17" s="3"/>
       <c r="AX17" s="3"/>
@@ -2249,32 +2228,26 @@
       <c r="BK17" s="3"/>
       <c r="BL17" s="3"/>
       <c r="BM17" s="3"/>
-      <c r="BN17" s="3"/>
     </row>
-    <row r="20" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20"/>
     </row>
-    <row r="22" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:65" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
     </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="K23" t="s">
-        <v>80</v>
+    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
         <v>50</v>
       </c>
-      <c r="J25" t="s">
+      <c r="I25" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="I27" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove serviceWorker from matrix, as it is not a class and served no user story directly (AFAIK)
</commit_message>
<xml_diff>
--- a/6- Traceability link matrix/Traceability Link Matrix (P3).xlsx
+++ b/6- Traceability link matrix/Traceability Link Matrix (P3).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\CS414 Group Project\cs414-f20-public_class_TeamD\6- Traceability link matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCBFF45-FCDA-4CFD-B45E-121628C9C769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC1FE37-116F-4C8F-B4AB-441BDCA11A03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44475" yWindow="4740" windowWidth="26400" windowHeight="11385" xr2:uid="{6F3B0F6D-D4FA-43ED-9BE5-68FBBAC2F32D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="79">
   <si>
     <t>User Stories</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>index</t>
-  </si>
-  <si>
-    <t>serviceWorker</t>
   </si>
   <si>
     <t>CreateMatch</t>
@@ -650,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C21C376-BCAA-4BB5-9BB8-5CF377B37712}">
-  <dimension ref="A1:BM25"/>
+  <dimension ref="A1:BL25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
@@ -666,75 +663,74 @@
     <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="21" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="16" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="21" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -758,7 +754,7 @@
         <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
         <v>47</v>
@@ -767,7 +763,7 @@
         <v>48</v>
       </c>
       <c r="L2" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="M2" t="s">
         <v>25</v>
@@ -776,31 +772,31 @@
         <v>26</v>
       </c>
       <c r="O2" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="P2" t="s">
         <v>51</v>
       </c>
       <c r="Q2" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="R2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S2" t="s">
         <v>31</v>
       </c>
       <c r="T2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" t="s">
         <v>32</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
+        <v>52</v>
+      </c>
+      <c r="W2" t="s">
         <v>34</v>
-      </c>
-      <c r="V2" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" t="s">
-        <v>53</v>
       </c>
       <c r="X2" t="s">
         <v>35</v>
@@ -815,16 +811,16 @@
         <v>38</v>
       </c>
       <c r="AB2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AF2" t="s">
         <v>54</v>
@@ -836,40 +832,40 @@
         <v>56</v>
       </c>
       <c r="AI2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>57</v>
       </c>
-      <c r="AJ2" t="s">
-        <v>21</v>
-      </c>
       <c r="AK2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR2" t="s">
         <v>58</v>
       </c>
-      <c r="AL2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>40</v>
-      </c>
       <c r="AS2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT2" t="s">
         <v>59</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>44</v>
       </c>
       <c r="AU2" t="s">
         <v>60</v>
@@ -925,11 +921,8 @@
       <c r="BL2" t="s">
         <v>77</v>
       </c>
-      <c r="BM2" t="s">
-        <v>78</v>
-      </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -937,13 +930,13 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -953,10 +946,10 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="Q3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -979,23 +972,23 @@
       <c r="AL3" s="3"/>
       <c r="AM3" s="3"/>
       <c r="AN3" s="3"/>
-      <c r="AO3" s="3"/>
+      <c r="AO3" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AP3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AQ3" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AQ3" s="3"/>
       <c r="AR3" s="3"/>
-      <c r="AS3" s="3"/>
-      <c r="AT3" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AS3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT3" s="3"/>
       <c r="AU3" s="3"/>
-      <c r="AV3" s="3"/>
-      <c r="AW3" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AV3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW3" s="3"/>
       <c r="AX3" s="3"/>
       <c r="AY3" s="3"/>
       <c r="AZ3" s="3"/>
@@ -1005,16 +998,15 @@
       <c r="BD3" s="3"/>
       <c r="BE3" s="3"/>
       <c r="BF3" s="3"/>
-      <c r="BG3" s="3"/>
+      <c r="BH3" s="3"/>
       <c r="BI3" s="3"/>
       <c r="BJ3" s="3"/>
-      <c r="BK3" s="3"/>
-      <c r="BL3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BM3" s="3"/>
+      <c r="BK3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BL3" s="3"/>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1074,37 +1066,36 @@
       <c r="BD4" s="3"/>
       <c r="BE4" s="3"/>
       <c r="BF4" s="3"/>
-      <c r="BG4" s="3"/>
+      <c r="BH4" s="3"/>
       <c r="BI4" s="3"/>
       <c r="BJ4" s="3"/>
       <c r="BK4" s="3"/>
       <c r="BL4" s="3"/>
-      <c r="BM4" s="3"/>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="K5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -1131,20 +1122,20 @@
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
       <c r="AL5" s="3"/>
-      <c r="AM5" s="3"/>
+      <c r="AM5" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AN5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AO5" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AO5" s="3"/>
       <c r="AP5" s="3"/>
       <c r="AQ5" s="3"/>
       <c r="AR5" s="3"/>
-      <c r="AS5" s="3"/>
-      <c r="AT5" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AS5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT5" s="3"/>
       <c r="AU5" s="3"/>
       <c r="AV5" s="3"/>
       <c r="AW5" s="3"/>
@@ -1157,55 +1148,54 @@
       <c r="BD5" s="3"/>
       <c r="BE5" s="3"/>
       <c r="BF5" s="3"/>
-      <c r="BG5" s="3"/>
+      <c r="BH5" s="3"/>
       <c r="BI5" s="3"/>
       <c r="BJ5" s="3"/>
       <c r="BK5" s="3"/>
-      <c r="BL5" s="3"/>
-      <c r="BM5" s="3" t="s">
-        <v>46</v>
+      <c r="BL5" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="L6" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="M6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
@@ -1218,19 +1208,19 @@
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
+      <c r="AE6" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AF6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AG6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI6" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
       <c r="AK6" s="3"/>
       <c r="AL6" s="3"/>
@@ -1238,25 +1228,25 @@
       <c r="AN6" s="3"/>
       <c r="AO6" s="3"/>
       <c r="AP6" s="3"/>
-      <c r="AQ6" s="3"/>
+      <c r="AQ6" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AR6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AS6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AT6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AU6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AV6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AW6" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AW6" s="3"/>
       <c r="AX6" s="3"/>
       <c r="AY6" s="3"/>
       <c r="AZ6" s="3"/>
@@ -1266,55 +1256,54 @@
       <c r="BD6" s="3"/>
       <c r="BE6" s="3"/>
       <c r="BF6" s="3"/>
-      <c r="BG6" s="3"/>
-      <c r="BI6" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="BH6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BI6" s="3"/>
       <c r="BJ6" s="3"/>
       <c r="BK6" s="3"/>
       <c r="BL6" s="3"/>
-      <c r="BM6" s="3"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="L7" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="M7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -1327,19 +1316,19 @@
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
+      <c r="AE7" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AF7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AG7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI7" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
       <c r="AK7" s="3"/>
       <c r="AL7" s="3"/>
@@ -1349,19 +1338,19 @@
       <c r="AP7" s="3"/>
       <c r="AQ7" s="3"/>
       <c r="AR7" s="3"/>
-      <c r="AS7" s="3"/>
+      <c r="AS7" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AT7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AU7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AV7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AW7" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AW7" s="3"/>
       <c r="AX7" s="3"/>
       <c r="AY7" s="3"/>
       <c r="AZ7" s="3"/>
@@ -1371,16 +1360,15 @@
       <c r="BD7" s="3"/>
       <c r="BE7" s="3"/>
       <c r="BF7" s="3"/>
-      <c r="BG7" s="3"/>
-      <c r="BI7" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="BH7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BI7" s="3"/>
       <c r="BJ7" s="3"/>
       <c r="BK7" s="3"/>
       <c r="BL7" s="3"/>
-      <c r="BM7" s="3"/>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -1440,14 +1428,13 @@
       <c r="BD8" s="3"/>
       <c r="BE8" s="3"/>
       <c r="BF8" s="3"/>
-      <c r="BG8" s="3"/>
+      <c r="BH8" s="3"/>
       <c r="BI8" s="3"/>
       <c r="BJ8" s="3"/>
       <c r="BK8" s="3"/>
       <c r="BL8" s="3"/>
-      <c r="BM8" s="3"/>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1507,14 +1494,13 @@
       <c r="BD9" s="3"/>
       <c r="BE9" s="3"/>
       <c r="BF9" s="3"/>
-      <c r="BG9" s="3"/>
+      <c r="BH9" s="3"/>
       <c r="BI9" s="3"/>
       <c r="BJ9" s="3"/>
       <c r="BK9" s="3"/>
       <c r="BL9" s="3"/>
-      <c r="BM9" s="3"/>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -1522,13 +1508,13 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -1538,10 +1524,10 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="Q10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
@@ -1558,35 +1544,35 @@
       <c r="AF10" s="3"/>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
+      <c r="AI10" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AJ10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AK10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AL10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AM10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN10" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AN10" s="3"/>
       <c r="AO10" s="3"/>
       <c r="AP10" s="3"/>
       <c r="AQ10" s="3"/>
       <c r="AR10" s="3"/>
-      <c r="AS10" s="3"/>
-      <c r="AT10" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AS10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT10" s="3"/>
       <c r="AU10" s="3"/>
-      <c r="AV10" s="3"/>
-      <c r="AW10" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AV10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW10" s="3"/>
       <c r="AX10" s="3"/>
       <c r="AY10" s="3"/>
       <c r="AZ10" s="3"/>
@@ -1596,20 +1582,19 @@
       <c r="BD10" s="3"/>
       <c r="BE10" s="3"/>
       <c r="BF10" s="3"/>
-      <c r="BG10" s="3"/>
-      <c r="BI10" s="3"/>
+      <c r="BH10" s="3"/>
+      <c r="BI10" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="BJ10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BK10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BL10" s="3"/>
-      <c r="BM10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="BK10" s="3"/>
+      <c r="BL10" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -1617,61 +1602,61 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="J11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
+      <c r="Q11" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="R11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
+      <c r="Y11" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="Z11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AA11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AD11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE11" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AE11" s="3"/>
       <c r="AF11" s="3"/>
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
@@ -1685,68 +1670,67 @@
       <c r="AP11" s="3"/>
       <c r="AQ11" s="3"/>
       <c r="AR11" s="3"/>
-      <c r="AS11" s="3"/>
-      <c r="AT11" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AS11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT11" s="3"/>
       <c r="AU11" s="3"/>
-      <c r="AV11" s="3"/>
+      <c r="AV11" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AW11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AX11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AY11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AZ11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BA11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BB11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BC11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BD11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BE11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BF11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BG11" s="3"/>
-      <c r="BH11" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="BF11" s="3"/>
+      <c r="BG11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH11" s="3"/>
       <c r="BI11" s="3"/>
       <c r="BJ11" s="3"/>
       <c r="BK11" s="3"/>
       <c r="BL11" s="3"/>
-      <c r="BM11" s="3"/>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1799,14 +1783,13 @@
       <c r="BD12" s="3"/>
       <c r="BE12" s="3"/>
       <c r="BF12" s="3"/>
-      <c r="BG12" s="3"/>
+      <c r="BH12" s="3"/>
       <c r="BI12" s="3"/>
       <c r="BJ12" s="3"/>
       <c r="BK12" s="3"/>
       <c r="BL12" s="3"/>
-      <c r="BM12" s="3"/>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -1866,14 +1849,13 @@
       <c r="BD13" s="3"/>
       <c r="BE13" s="3"/>
       <c r="BF13" s="3"/>
-      <c r="BG13" s="3"/>
+      <c r="BH13" s="3"/>
       <c r="BI13" s="3"/>
       <c r="BJ13" s="3"/>
       <c r="BK13" s="3"/>
       <c r="BL13" s="3"/>
-      <c r="BM13" s="3"/>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -1881,10 +1863,10 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1921,16 +1903,16 @@
       <c r="AN14" s="3"/>
       <c r="AO14" s="3"/>
       <c r="AP14" s="3"/>
-      <c r="AQ14" s="3"/>
+      <c r="AQ14" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AR14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AS14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT14" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AT14" s="3"/>
       <c r="AU14" s="3"/>
       <c r="AV14" s="3"/>
       <c r="AW14" s="3"/>
@@ -1943,14 +1925,13 @@
       <c r="BD14" s="3"/>
       <c r="BE14" s="3"/>
       <c r="BF14" s="3"/>
-      <c r="BG14" s="3"/>
+      <c r="BH14" s="3"/>
       <c r="BI14" s="3"/>
       <c r="BJ14" s="3"/>
       <c r="BK14" s="3"/>
       <c r="BL14" s="3"/>
-      <c r="BM14" s="3"/>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -1958,65 +1939,65 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="I15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
+      <c r="Q15" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="R15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="X15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Y15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AA15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AB15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AD15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE15" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
@@ -2030,55 +2011,54 @@
       <c r="AP15" s="3"/>
       <c r="AQ15" s="3"/>
       <c r="AR15" s="3"/>
-      <c r="AS15" s="3"/>
-      <c r="AT15" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AS15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT15" s="3"/>
       <c r="AU15" s="3"/>
-      <c r="AV15" s="3"/>
+      <c r="AV15" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AW15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AX15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AY15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AZ15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BA15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BB15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BC15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BD15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BE15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BF15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="BG15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BH15" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="BH15" s="3"/>
       <c r="BI15" s="3"/>
       <c r="BJ15" s="3"/>
       <c r="BK15" s="3"/>
       <c r="BL15" s="3"/>
-      <c r="BM15" s="3"/>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -2088,10 +2068,10 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="I16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -2101,17 +2081,17 @@
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="T16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="U16" s="3"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="Y16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
@@ -2130,34 +2110,33 @@
       <c r="AP16" s="3"/>
       <c r="AQ16" s="3"/>
       <c r="AR16" s="3"/>
-      <c r="AS16" s="3"/>
-      <c r="AT16" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AS16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT16" s="3"/>
       <c r="AU16" s="3"/>
       <c r="AV16" s="3"/>
       <c r="AW16" s="3"/>
       <c r="AX16" s="3"/>
-      <c r="AY16" s="3"/>
-      <c r="AZ16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BA16" s="3"/>
-      <c r="BB16" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AY16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ16" s="3"/>
+      <c r="BA16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB16" s="3"/>
       <c r="BC16" s="3"/>
       <c r="BD16" s="3"/>
       <c r="BE16" s="3"/>
       <c r="BF16" s="3"/>
-      <c r="BG16" s="3"/>
+      <c r="BH16" s="3"/>
       <c r="BI16" s="3"/>
       <c r="BJ16" s="3"/>
       <c r="BK16" s="3"/>
       <c r="BL16" s="3"/>
-      <c r="BM16" s="3"/>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -2167,10 +2146,10 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="I17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -2205,10 +2184,10 @@
       <c r="AP17" s="3"/>
       <c r="AQ17" s="3"/>
       <c r="AR17" s="3"/>
-      <c r="AS17" s="3"/>
-      <c r="AT17" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AS17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT17" s="3"/>
       <c r="AU17" s="3"/>
       <c r="AV17" s="3"/>
       <c r="AW17" s="3"/>
@@ -2227,27 +2206,23 @@
       <c r="BJ17" s="3"/>
       <c r="BK17" s="3"/>
       <c r="BL17" s="3"/>
-      <c r="BM17" s="3"/>
     </row>
-    <row r="20" spans="1:65" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20"/>
     </row>
-    <row r="22" spans="1:65" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="J23" t="s">
-        <v>79</v>
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update TLM with classes from "crunch time"
</commit_message>
<xml_diff>
--- a/6- Traceability link matrix/Traceability Link Matrix (P3).xlsx
+++ b/6- Traceability link matrix/Traceability Link Matrix (P3).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\CS414 Group Project\cs414-f20-public_class_TeamD\6- Traceability link matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A1D078-63F7-4601-97E9-B86D67BB00FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC2827E-0E7B-4E1B-AA28-51A287457C3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44475" yWindow="4740" windowWidth="26400" windowHeight="11385" xr2:uid="{6F3B0F6D-D4FA-43ED-9BE5-68FBBAC2F32D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F3B0F6D-D4FA-43ED-9BE5-68FBBAC2F32D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="82">
   <si>
     <t>User Stories</t>
   </si>
@@ -268,6 +268,18 @@
   </si>
   <si>
     <t>OngoingMatchesTest</t>
+  </si>
+  <si>
+    <t>MatchHistory</t>
+  </si>
+  <si>
+    <t>GameplayController</t>
+  </si>
+  <si>
+    <t>MovePiece</t>
+  </si>
+  <si>
+    <t>MatchHistoryController</t>
   </si>
 </sst>
 </file>
@@ -644,11 +656,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C21C376-BCAA-4BB5-9BB8-5CF377B37712}">
-  <dimension ref="A1:BL22"/>
+  <dimension ref="A1:BQ22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G20" sqref="G20"/>
+      <selection pane="topRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,78 +668,83 @@
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="21" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="21" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="16" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="10" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -739,203 +756,218 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>46</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>47</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>48</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>25</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>50</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>51</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>27</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>30</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>31</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>33</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>32</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X2" t="s">
         <v>52</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>34</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>36</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD2" t="s">
         <v>38</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AE2" t="s">
         <v>40</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AF2" t="s">
         <v>42</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AG2" t="s">
         <v>44</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AH2" t="s">
         <v>53</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AI2" t="s">
         <v>54</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AJ2" t="s">
         <v>55</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AK2" t="s">
         <v>56</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AL2" t="s">
         <v>21</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AM2" t="s">
         <v>57</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AN2" t="s">
         <v>9</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AO2" t="s">
         <v>28</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AP2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR2" t="s">
         <v>20</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AS2" t="s">
         <v>29</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AT2" t="s">
         <v>2</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AU2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AV2" t="s">
         <v>39</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AW2" t="s">
         <v>58</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AX2" t="s">
         <v>43</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AY2" t="s">
         <v>59</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AZ2" t="s">
         <v>60</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="BA2" t="s">
         <v>61</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="BB2" t="s">
         <v>62</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="BC2" t="s">
         <v>63</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BD2" t="s">
         <v>64</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BE2" t="s">
         <v>65</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BF2" t="s">
         <v>66</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BG2" t="s">
         <v>67</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BH2" t="s">
         <v>68</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BI2" t="s">
         <v>69</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BJ2" t="s">
         <v>70</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BK2" t="s">
         <v>71</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BL2" t="s">
         <v>72</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BM2" t="s">
         <v>73</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="BN2" t="s">
         <v>74</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="BO2" t="s">
         <v>75</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="BP2" t="s">
         <v>76</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BQ2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -943,10 +975,10 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -969,41 +1001,46 @@
       <c r="AL3" s="3"/>
       <c r="AM3" s="3"/>
       <c r="AN3" s="3"/>
-      <c r="AO3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AP3" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AO3" s="3"/>
+      <c r="AP3" s="3"/>
       <c r="AQ3" s="3"/>
       <c r="AR3" s="3"/>
-      <c r="AS3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AT3" s="3"/>
-      <c r="AU3" s="3"/>
-      <c r="AV3" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AS3" s="3"/>
+      <c r="AT3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV3" s="3"/>
       <c r="AW3" s="3"/>
-      <c r="AX3" s="3"/>
+      <c r="AX3" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AY3" s="3"/>
       <c r="AZ3" s="3"/>
-      <c r="BA3" s="3"/>
+      <c r="BA3" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="BB3" s="3"/>
       <c r="BC3" s="3"/>
       <c r="BD3" s="3"/>
       <c r="BE3" s="3"/>
       <c r="BF3" s="3"/>
+      <c r="BG3" s="3"/>
       <c r="BH3" s="3"/>
       <c r="BI3" s="3"/>
       <c r="BJ3" s="3"/>
-      <c r="BK3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="BL3" s="3"/>
+      <c r="BK3" s="3"/>
+      <c r="BM3" s="3"/>
+      <c r="BN3" s="3"/>
+      <c r="BO3" s="3"/>
+      <c r="BP3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BQ3" s="3"/>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1063,13 +1100,18 @@
       <c r="BD4" s="3"/>
       <c r="BE4" s="3"/>
       <c r="BF4" s="3"/>
+      <c r="BG4" s="3"/>
       <c r="BH4" s="3"/>
       <c r="BI4" s="3"/>
       <c r="BJ4" s="3"/>
       <c r="BK4" s="3"/>
-      <c r="BL4" s="3"/>
+      <c r="BM4" s="3"/>
+      <c r="BN4" s="3"/>
+      <c r="BO4" s="3"/>
+      <c r="BP4" s="3"/>
+      <c r="BQ4" s="3"/>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1086,13 +1128,15 @@
       <c r="G5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -1119,16 +1163,18 @@
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
       <c r="AL5" s="3"/>
-      <c r="AM5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AN5" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
       <c r="AO5" s="3"/>
-      <c r="AP5" s="3"/>
-      <c r="AQ5" s="3"/>
-      <c r="AR5" s="3"/>
+      <c r="AP5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AR5" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AS5" s="3" t="s">
         <v>45</v>
       </c>
@@ -1136,7 +1182,9 @@
       <c r="AU5" s="3"/>
       <c r="AV5" s="3"/>
       <c r="AW5" s="3"/>
-      <c r="AX5" s="3"/>
+      <c r="AX5" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AY5" s="3"/>
       <c r="AZ5" s="3"/>
       <c r="BA5" s="3"/>
@@ -1145,15 +1193,20 @@
       <c r="BD5" s="3"/>
       <c r="BE5" s="3"/>
       <c r="BF5" s="3"/>
+      <c r="BG5" s="3"/>
       <c r="BH5" s="3"/>
       <c r="BI5" s="3"/>
       <c r="BJ5" s="3"/>
       <c r="BK5" s="3"/>
-      <c r="BL5" s="3" t="s">
+      <c r="BM5" s="3"/>
+      <c r="BN5" s="3"/>
+      <c r="BO5" s="3"/>
+      <c r="BP5" s="3"/>
+      <c r="BQ5" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1161,22 +1214,20 @@
         <v>45</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="L6" s="3"/>
       <c r="M6" s="3" t="s">
         <v>45</v>
       </c>
@@ -1192,7 +1243,9 @@
       <c r="Q6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="3"/>
+      <c r="R6" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
@@ -1205,63 +1258,68 @@
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG6" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
       <c r="AH6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AI6" s="3"/>
-      <c r="AJ6" s="3"/>
-      <c r="AK6" s="3"/>
+      <c r="AI6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AL6" s="3"/>
       <c r="AM6" s="3"/>
       <c r="AN6" s="3"/>
       <c r="AO6" s="3"/>
       <c r="AP6" s="3"/>
-      <c r="AQ6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AR6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AT6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU6" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+      <c r="AU6" s="3"/>
       <c r="AV6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AW6" s="3"/>
-      <c r="AX6" s="3"/>
-      <c r="AY6" s="3"/>
-      <c r="AZ6" s="3"/>
-      <c r="BA6" s="3"/>
+      <c r="AW6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AX6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA6" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="BB6" s="3"/>
       <c r="BC6" s="3"/>
       <c r="BD6" s="3"/>
       <c r="BE6" s="3"/>
       <c r="BF6" s="3"/>
-      <c r="BH6" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="BG6" s="3"/>
+      <c r="BH6" s="3"/>
       <c r="BI6" s="3"/>
       <c r="BJ6" s="3"/>
       <c r="BK6" s="3"/>
-      <c r="BL6" s="3"/>
+      <c r="BM6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BN6" s="3"/>
+      <c r="BO6" s="3"/>
+      <c r="BP6" s="3"/>
+      <c r="BQ6" s="3"/>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -1269,22 +1327,20 @@
         <v>45</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="L7" s="3"/>
       <c r="M7" s="3" t="s">
         <v>45</v>
       </c>
@@ -1300,7 +1356,9 @@
       <c r="Q7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="R7" s="3"/>
+      <c r="R7" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -1313,21 +1371,21 @@
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
-      <c r="AE7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG7" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
       <c r="AH7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AI7" s="3"/>
-      <c r="AJ7" s="3"/>
-      <c r="AK7" s="3"/>
+      <c r="AI7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK7" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AL7" s="3"/>
       <c r="AM7" s="3"/>
       <c r="AN7" s="3"/>
@@ -1335,37 +1393,42 @@
       <c r="AP7" s="3"/>
       <c r="AQ7" s="3"/>
       <c r="AR7" s="3"/>
-      <c r="AS7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AT7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV7" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+      <c r="AU7" s="3"/>
+      <c r="AV7" s="3"/>
       <c r="AW7" s="3"/>
-      <c r="AX7" s="3"/>
-      <c r="AY7" s="3"/>
-      <c r="AZ7" s="3"/>
-      <c r="BA7" s="3"/>
+      <c r="AX7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA7" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="BB7" s="3"/>
       <c r="BC7" s="3"/>
       <c r="BD7" s="3"/>
       <c r="BE7" s="3"/>
       <c r="BF7" s="3"/>
-      <c r="BH7" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="BG7" s="3"/>
+      <c r="BH7" s="3"/>
       <c r="BI7" s="3"/>
       <c r="BJ7" s="3"/>
       <c r="BK7" s="3"/>
-      <c r="BL7" s="3"/>
+      <c r="BM7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BN7" s="3"/>
+      <c r="BO7" s="3"/>
+      <c r="BP7" s="3"/>
+      <c r="BQ7" s="3"/>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -1425,13 +1488,18 @@
       <c r="BD8" s="3"/>
       <c r="BE8" s="3"/>
       <c r="BF8" s="3"/>
+      <c r="BG8" s="3"/>
       <c r="BH8" s="3"/>
       <c r="BI8" s="3"/>
       <c r="BJ8" s="3"/>
       <c r="BK8" s="3"/>
-      <c r="BL8" s="3"/>
+      <c r="BM8" s="3"/>
+      <c r="BN8" s="3"/>
+      <c r="BO8" s="3"/>
+      <c r="BP8" s="3"/>
+      <c r="BQ8" s="3"/>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1491,29 +1559,34 @@
       <c r="BD9" s="3"/>
       <c r="BE9" s="3"/>
       <c r="BF9" s="3"/>
+      <c r="BG9" s="3"/>
       <c r="BH9" s="3"/>
       <c r="BI9" s="3"/>
       <c r="BJ9" s="3"/>
       <c r="BK9" s="3"/>
-      <c r="BL9" s="3"/>
+      <c r="BM9" s="3"/>
+      <c r="BN9" s="3"/>
+      <c r="BO9" s="3"/>
+      <c r="BP9" s="3"/>
+      <c r="BQ9" s="3"/>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -1521,10 +1594,10 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
@@ -1541,85 +1614,88 @@
       <c r="AF10" s="3"/>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
-      <c r="AI10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK10" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
       <c r="AL10" s="3" t="s">
         <v>45</v>
       </c>
       <c r="AM10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AN10" s="3"/>
-      <c r="AO10" s="3"/>
+      <c r="AN10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO10" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AP10" s="3"/>
       <c r="AQ10" s="3"/>
-      <c r="AR10" s="3"/>
-      <c r="AS10" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AR10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS10" s="3"/>
       <c r="AT10" s="3"/>
       <c r="AU10" s="3"/>
-      <c r="AV10" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AV10" s="3"/>
       <c r="AW10" s="3"/>
-      <c r="AX10" s="3"/>
+      <c r="AX10" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AY10" s="3"/>
       <c r="AZ10" s="3"/>
-      <c r="BA10" s="3"/>
+      <c r="BA10" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="BB10" s="3"/>
       <c r="BC10" s="3"/>
       <c r="BD10" s="3"/>
       <c r="BE10" s="3"/>
       <c r="BF10" s="3"/>
+      <c r="BG10" s="3"/>
       <c r="BH10" s="3"/>
-      <c r="BI10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="BJ10" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="BI10" s="3"/>
+      <c r="BJ10" s="3"/>
       <c r="BK10" s="3"/>
-      <c r="BL10" s="3" t="s">
+      <c r="BM10" s="3"/>
+      <c r="BN10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BO10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BP10" s="3"/>
+      <c r="BQ10" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="H11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="K11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="Q11" s="3"/>
       <c r="R11" s="3" t="s">
         <v>45</v>
       </c>
@@ -1632,30 +1708,34 @@
       <c r="U11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
+      <c r="V11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="X11" s="3"/>
-      <c r="Y11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
       <c r="AA11" s="3" t="s">
         <v>45</v>
       </c>
       <c r="AB11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AC11" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AC11" s="3"/>
       <c r="AD11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AE11" s="3"/>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
+      <c r="AE11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG11" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AH11" s="3"/>
       <c r="AI11" s="3"/>
       <c r="AJ11" s="3"/>
@@ -1667,26 +1747,16 @@
       <c r="AP11" s="3"/>
       <c r="AQ11" s="3"/>
       <c r="AR11" s="3"/>
-      <c r="AS11" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AS11" s="3"/>
       <c r="AT11" s="3"/>
       <c r="AU11" s="3"/>
-      <c r="AV11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AW11" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AV11" s="3"/>
+      <c r="AW11" s="3"/>
       <c r="AX11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AY11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AZ11" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AY11" s="3"/>
+      <c r="AZ11" s="3"/>
       <c r="BA11" s="3" t="s">
         <v>45</v>
       </c>
@@ -1702,17 +1772,32 @@
       <c r="BE11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="BF11" s="3"/>
+      <c r="BF11" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="BG11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="BH11" s="3"/>
-      <c r="BI11" s="3"/>
-      <c r="BJ11" s="3"/>
+      <c r="BH11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BI11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BJ11" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="BK11" s="3"/>
-      <c r="BL11" s="3"/>
+      <c r="BL11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BM11" s="3"/>
+      <c r="BN11" s="3"/>
+      <c r="BO11" s="3"/>
+      <c r="BP11" s="3"/>
+      <c r="BQ11" s="3"/>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -1729,7 +1814,9 @@
       <c r="G12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1744,7 +1831,9 @@
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
+      <c r="W12" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
@@ -1763,8 +1852,12 @@
       <c r="AM12" s="3"/>
       <c r="AN12" s="3"/>
       <c r="AO12" s="3"/>
-      <c r="AP12" s="3"/>
-      <c r="AQ12" s="3"/>
+      <c r="AP12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ12" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AR12" s="3"/>
       <c r="AS12" s="3"/>
       <c r="AT12" s="3"/>
@@ -1780,13 +1873,18 @@
       <c r="BD12" s="3"/>
       <c r="BE12" s="3"/>
       <c r="BF12" s="3"/>
+      <c r="BG12" s="3"/>
       <c r="BH12" s="3"/>
       <c r="BI12" s="3"/>
       <c r="BJ12" s="3"/>
       <c r="BK12" s="3"/>
-      <c r="BL12" s="3"/>
+      <c r="BM12" s="3"/>
+      <c r="BN12" s="3"/>
+      <c r="BO12" s="3"/>
+      <c r="BP12" s="3"/>
+      <c r="BQ12" s="3"/>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -1846,26 +1944,31 @@
       <c r="BD13" s="3"/>
       <c r="BE13" s="3"/>
       <c r="BF13" s="3"/>
+      <c r="BG13" s="3"/>
       <c r="BH13" s="3"/>
       <c r="BI13" s="3"/>
       <c r="BJ13" s="3"/>
       <c r="BK13" s="3"/>
-      <c r="BL13" s="3"/>
+      <c r="BM13" s="3"/>
+      <c r="BN13" s="3"/>
+      <c r="BO13" s="3"/>
+      <c r="BP13" s="3"/>
+      <c r="BQ13" s="3"/>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1880,7 +1983,9 @@
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
+      <c r="W14" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
@@ -1900,20 +2005,20 @@
       <c r="AN14" s="3"/>
       <c r="AO14" s="3"/>
       <c r="AP14" s="3"/>
-      <c r="AQ14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AR14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS14" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AQ14" s="3"/>
+      <c r="AR14" s="3"/>
+      <c r="AS14" s="3"/>
       <c r="AT14" s="3"/>
       <c r="AU14" s="3"/>
-      <c r="AV14" s="3"/>
-      <c r="AW14" s="3"/>
-      <c r="AX14" s="3"/>
+      <c r="AV14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AX14" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AY14" s="3"/>
       <c r="AZ14" s="3"/>
       <c r="BA14" s="3"/>
@@ -1922,39 +2027,42 @@
       <c r="BD14" s="3"/>
       <c r="BE14" s="3"/>
       <c r="BF14" s="3"/>
+      <c r="BG14" s="3"/>
       <c r="BH14" s="3"/>
       <c r="BI14" s="3"/>
       <c r="BJ14" s="3"/>
       <c r="BK14" s="3"/>
-      <c r="BL14" s="3"/>
+      <c r="BM14" s="3"/>
+      <c r="BN14" s="3"/>
+      <c r="BO14" s="3"/>
+      <c r="BP14" s="3"/>
+      <c r="BQ14" s="3"/>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="Q15" s="3"/>
       <c r="R15" s="3" t="s">
         <v>45</v>
       </c>
@@ -1994,9 +2102,15 @@
       <c r="AD15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AE15" s="3"/>
-      <c r="AF15" s="3"/>
-      <c r="AG15" s="3"/>
+      <c r="AE15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG15" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AH15" s="3"/>
       <c r="AI15" s="3"/>
       <c r="AJ15" s="3"/>
@@ -2008,26 +2122,16 @@
       <c r="AP15" s="3"/>
       <c r="AQ15" s="3"/>
       <c r="AR15" s="3"/>
-      <c r="AS15" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AS15" s="3"/>
       <c r="AT15" s="3"/>
       <c r="AU15" s="3"/>
-      <c r="AV15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AW15" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AV15" s="3"/>
+      <c r="AW15" s="3"/>
       <c r="AX15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AY15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AZ15" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AY15" s="3"/>
+      <c r="AZ15" s="3"/>
       <c r="BA15" s="3" t="s">
         <v>45</v>
       </c>
@@ -2049,13 +2153,28 @@
       <c r="BG15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="BH15" s="3"/>
-      <c r="BI15" s="3"/>
-      <c r="BJ15" s="3"/>
-      <c r="BK15" s="3"/>
-      <c r="BL15" s="3"/>
+      <c r="BH15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BI15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BJ15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BK15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BL15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BM15" s="3"/>
+      <c r="BN15" s="3"/>
+      <c r="BO15" s="3"/>
+      <c r="BP15" s="3"/>
+      <c r="BQ15" s="3"/>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -2065,10 +2184,10 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -2078,18 +2197,20 @@
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
-      <c r="T16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="U16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
+      <c r="W16" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="X16" s="3"/>
-      <c r="Y16" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
+      <c r="AA16" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
@@ -2107,33 +2228,38 @@
       <c r="AP16" s="3"/>
       <c r="AQ16" s="3"/>
       <c r="AR16" s="3"/>
-      <c r="AS16" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AS16" s="3"/>
       <c r="AT16" s="3"/>
       <c r="AU16" s="3"/>
       <c r="AV16" s="3"/>
       <c r="AW16" s="3"/>
-      <c r="AX16" s="3"/>
-      <c r="AY16" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AX16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY16" s="3"/>
       <c r="AZ16" s="3"/>
-      <c r="BA16" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="BA16" s="3"/>
       <c r="BB16" s="3"/>
       <c r="BC16" s="3"/>
-      <c r="BD16" s="3"/>
+      <c r="BD16" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="BE16" s="3"/>
-      <c r="BF16" s="3"/>
+      <c r="BF16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BG16" s="3"/>
       <c r="BH16" s="3"/>
       <c r="BI16" s="3"/>
       <c r="BJ16" s="3"/>
       <c r="BK16" s="3"/>
-      <c r="BL16" s="3"/>
+      <c r="BM16" s="3"/>
+      <c r="BN16" s="3"/>
+      <c r="BO16" s="3"/>
+      <c r="BP16" s="3"/>
+      <c r="BQ16" s="3"/>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -2143,10 +2269,10 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -2181,14 +2307,14 @@
       <c r="AP17" s="3"/>
       <c r="AQ17" s="3"/>
       <c r="AR17" s="3"/>
-      <c r="AS17" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="AS17" s="3"/>
       <c r="AT17" s="3"/>
       <c r="AU17" s="3"/>
       <c r="AV17" s="3"/>
       <c r="AW17" s="3"/>
-      <c r="AX17" s="3"/>
+      <c r="AX17" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="AY17" s="3"/>
       <c r="AZ17" s="3"/>
       <c r="BA17" s="3"/>
@@ -2203,17 +2329,22 @@
       <c r="BJ17" s="3"/>
       <c r="BK17" s="3"/>
       <c r="BL17" s="3"/>
+      <c r="BM17" s="3"/>
+      <c r="BN17" s="3"/>
+      <c r="BO17" s="3"/>
+      <c r="BP17" s="3"/>
+      <c r="BQ17" s="3"/>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="G19" t="s">
+    <row r="19" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
     </row>

</xml_diff>

<commit_message>
corrected tlm for database.java
</commit_message>
<xml_diff>
--- a/6- Traceability link matrix/Traceability Link Matrix (P3).xlsx
+++ b/6- Traceability link matrix/Traceability Link Matrix (P3).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\CS414 Group Project\cs414-f20-public_class_TeamD\6- Traceability link matrix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lakot\IdeaProjects\cs414-f20-public_class_TeamD\6- Traceability link matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC2827E-0E7B-4E1B-AA28-51A287457C3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DD0F09-31EA-41F1-A911-4017188E6336}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F3B0F6D-D4FA-43ED-9BE5-68FBBAC2F32D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{6F3B0F6D-D4FA-43ED-9BE5-68FBBAC2F32D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="82">
   <si>
     <t>User Stories</t>
   </si>
@@ -659,81 +658,81 @@
   <dimension ref="A1:BQ22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C3" sqref="C3"/>
+      <pane xSplit="2" topLeftCell="BE1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.68359375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.26171875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.68359375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26171875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.15625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.41796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.68359375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.15625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.83984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.26171875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.15625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.41796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.83984375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.83984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.68359375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.83984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.83984375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="7" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.41796875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.15625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.15625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.26171875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.83984375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.68359375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.83984375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22.15625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="16" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25.26171875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.68359375" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="21" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="6.578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.15625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="17.578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.83984375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15.15625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="14.83984375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="8.578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.578125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="10.83984375" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="16" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="10" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.41796875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="19.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,7 +743,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -951,7 +950,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1040,7 +1039,7 @@
       </c>
       <c r="BQ3" s="3"/>
     </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1111,7 +1110,7 @@
       <c r="BP4" s="3"/>
       <c r="BQ4" s="3"/>
     </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1142,7 +1141,9 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+      <c r="R5" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
@@ -1206,7 +1207,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1319,7 +1320,7 @@
       <c r="BP6" s="3"/>
       <c r="BQ6" s="3"/>
     </row>
-    <row r="7" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -1428,7 +1429,7 @@
       <c r="BP7" s="3"/>
       <c r="BQ7" s="3"/>
     </row>
-    <row r="8" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -1499,7 +1500,7 @@
       <c r="BP8" s="3"/>
       <c r="BQ8" s="3"/>
     </row>
-    <row r="9" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1570,7 +1571,7 @@
       <c r="BP9" s="3"/>
       <c r="BQ9" s="3"/>
     </row>
-    <row r="10" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -1669,7 +1670,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -1797,7 +1798,7 @@
       <c r="BP11" s="3"/>
       <c r="BQ11" s="3"/>
     </row>
-    <row r="12" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -1826,7 +1827,9 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
+      <c r="R12" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
@@ -1884,7 +1887,7 @@
       <c r="BP12" s="3"/>
       <c r="BQ12" s="3"/>
     </row>
-    <row r="13" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -1955,7 +1958,7 @@
       <c r="BP13" s="3"/>
       <c r="BQ13" s="3"/>
     </row>
-    <row r="14" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -1978,7 +1981,9 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
+      <c r="R14" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
@@ -2038,7 +2043,7 @@
       <c r="BP14" s="3"/>
       <c r="BQ14" s="3"/>
     </row>
-    <row r="15" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -2174,7 +2179,7 @@
       <c r="BP15" s="3"/>
       <c r="BQ15" s="3"/>
     </row>
-    <row r="16" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -2259,7 +2264,7 @@
       <c r="BP16" s="3"/>
       <c r="BQ16" s="3"/>
     </row>
-    <row r="17" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -2280,7 +2285,9 @@
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
+      <c r="R17" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
@@ -2335,16 +2342,16 @@
       <c r="BP17" s="3"/>
       <c r="BQ17" s="3"/>
     </row>
-    <row r="19" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:69" x14ac:dyDescent="0.55000000000000004">
       <c r="H19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20"/>
       <c r="B20"/>
     </row>
-    <row r="22" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22"/>
       <c r="B22"/>
     </row>

</xml_diff>